<commit_message>
Fix thêm excel phụ kiện next
</commit_message>
<xml_diff>
--- a/src/main/resources/report_templates/EXCEL_TO_PRODUCTION_PRODUCT.xlsx
+++ b/src/main/resources/report_templates/EXCEL_TO_PRODUCTION_PRODUCT.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\MeuPro\MeUVipPro\src\main\resources\report_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3CC0CE1-01D0-4E1C-95B5-3E37A57508BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7DA8A53-AF2D-4D66-AA05-5CCB6D72E6B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Trang_tính1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="ql0egwlKeIuqATQSjatGVj99bnNJqASTPSYUB8ze+Jc="/>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="55">
   <si>
     <t>1. KHO HÀNG CHỜ SẢN XUẤT: Bao gồm các trường sau</t>
   </si>
@@ -213,10 +213,6 @@
     <t>NV20241111</t>
   </si>
   <si>
-    <t xml:space="preserve">NBL0170
-</t>
-  </si>
-  <si>
     <t>PPT</t>
   </si>
   <si>
@@ -244,10 +240,6 @@
     <t>Mới</t>
   </si>
   <si>
-    <t xml:space="preserve">NBL0171
-</t>
-  </si>
-  <si>
     <t>Bánh phụ</t>
   </si>
   <si>
@@ -258,22 +250,6 @@
   </si>
   <si>
     <t>Đại lý B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NBL0172
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NBL0173
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NBL0174
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NBL0175
-</t>
   </si>
   <si>
     <t>Đại lý C</t>
@@ -382,7 +358,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -453,11 +429,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -491,6 +480,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -709,7 +702,7 @@
   <dimension ref="A1:AA999"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -718,7 +711,7 @@
     <col min="2" max="3" width="19.88671875" customWidth="1"/>
     <col min="4" max="4" width="25.77734375" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="8.6640625" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" customWidth="1"/>
     <col min="7" max="7" width="13.44140625" customWidth="1"/>
     <col min="8" max="8" width="17.44140625" customWidth="1"/>
     <col min="9" max="9" width="8.6640625" customWidth="1"/>
@@ -746,7 +739,7 @@
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -781,10 +774,10 @@
         <v>3</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>4</v>
@@ -838,10 +831,10 @@
         <v>20</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="Y2" s="3" t="s">
         <v>21</v>
@@ -854,66 +847,67 @@
       </c>
     </row>
     <row r="3" spans="1:27" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="8">
+      <c r="B3" s="14" t="str">
+        <f ca="1">"XE_"&amp;TEXT(RANDBETWEEN(0,99999),"00000")</f>
+        <v>XE_63789</v>
+      </c>
+      <c r="C3" s="13">
         <v>45570</v>
       </c>
       <c r="D3" s="8">
         <v>45576</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="F3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>27</v>
-      </c>
       <c r="H3" s="6" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="I3" s="6">
         <v>1500</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="K3" s="12">
         <v>100</v>
       </c>
       <c r="L3" s="6"/>
       <c r="M3" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="O3" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="O3" s="7" t="s">
+      <c r="P3" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="P3" s="7" t="s">
+      <c r="Q3" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="Q3" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="R3" s="6">
         <v>3</v>
       </c>
       <c r="S3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="T3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="U3" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="T3" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="U3" s="6" t="s">
-        <v>34</v>
       </c>
       <c r="V3" s="6">
         <v>100000</v>
@@ -925,7 +919,7 @@
         <v>120000</v>
       </c>
       <c r="Y3" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="Z3" s="6">
         <v>150000</v>
@@ -933,64 +927,65 @@
       <c r="AA3" s="6"/>
     </row>
     <row r="4" spans="1:27" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="8">
+      <c r="B4" s="14" t="str">
+        <f t="shared" ref="B4:B8" ca="1" si="0">"XE_"&amp;TEXT(RANDBETWEEN(0,99999),"00000")</f>
+        <v>XE_35376</v>
+      </c>
+      <c r="C4" s="13">
         <v>45571</v>
       </c>
       <c r="D4" s="8">
         <v>45576</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="F4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>27</v>
-      </c>
       <c r="H4" s="6" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="I4" s="6">
         <v>1500</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="K4" s="12">
         <v>100</v>
       </c>
       <c r="L4" s="6"/>
       <c r="M4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="N4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="N4" s="6" t="s">
+      <c r="O4" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="O4" s="7" t="s">
+      <c r="P4" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="P4" s="7" t="s">
+      <c r="Q4" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="Q4" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="R4" s="6"/>
       <c r="S4" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="T4" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="U4" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="V4" s="6">
         <v>100000</v>
@@ -1002,7 +997,7 @@
         <v>120000</v>
       </c>
       <c r="Y4" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="Z4" s="6">
         <v>150000</v>
@@ -1010,64 +1005,65 @@
       <c r="AA4" s="6"/>
     </row>
     <row r="5" spans="1:27" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="8">
+      <c r="B5" s="14" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>XE_91598</v>
+      </c>
+      <c r="C5" s="13">
         <v>45572</v>
       </c>
       <c r="D5" s="8">
         <v>45576</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="F5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="7" t="s">
-        <v>27</v>
-      </c>
       <c r="H5" s="6" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="I5" s="6">
         <v>1500</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="K5" s="12">
         <v>100</v>
       </c>
       <c r="L5" s="6"/>
       <c r="M5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="N5" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="N5" s="6" t="s">
+      <c r="O5" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="O5" s="7" t="s">
+      <c r="P5" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="P5" s="7" t="s">
+      <c r="Q5" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="Q5" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="R5" s="6"/>
       <c r="S5" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="T5" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="U5" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="V5" s="6">
         <v>100000</v>
@@ -1079,7 +1075,7 @@
         <v>120000</v>
       </c>
       <c r="Y5" s="6" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="Z5" s="6">
         <v>150000</v>
@@ -1087,64 +1083,65 @@
       <c r="AA5" s="6"/>
     </row>
     <row r="6" spans="1:27" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="8">
+      <c r="B6" s="14" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>XE_79877</v>
+      </c>
+      <c r="C6" s="13">
         <v>45573</v>
       </c>
       <c r="D6" s="8">
         <v>45576</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="F6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="7" t="s">
-        <v>27</v>
-      </c>
       <c r="H6" s="6" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="I6" s="6">
         <v>1500</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="K6" s="12">
         <v>100</v>
       </c>
       <c r="L6" s="6"/>
       <c r="M6" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="N6" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="N6" s="6" t="s">
+      <c r="O6" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="O6" s="7" t="s">
+      <c r="P6" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="P6" s="7" t="s">
+      <c r="Q6" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="Q6" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="R6" s="6"/>
       <c r="S6" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="T6" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="U6" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="V6" s="6">
         <v>100000</v>
@@ -1156,7 +1153,7 @@
         <v>120000</v>
       </c>
       <c r="Y6" s="6" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="Z6" s="6">
         <v>150000</v>
@@ -1164,64 +1161,65 @@
       <c r="AA6" s="6"/>
     </row>
     <row r="7" spans="1:27" s="10" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="8">
+      <c r="B7" s="14" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>XE_03503</v>
+      </c>
+      <c r="C7" s="13">
         <v>45574</v>
       </c>
       <c r="D7" s="8">
         <v>45576</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="F7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="7" t="s">
-        <v>27</v>
-      </c>
       <c r="H7" s="6" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="I7" s="6">
         <v>1500</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="K7" s="12">
         <v>100</v>
       </c>
       <c r="L7" s="6"/>
       <c r="M7" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="N7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="N7" s="6" t="s">
+      <c r="O7" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="O7" s="7" t="s">
+      <c r="P7" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="P7" s="7" t="s">
+      <c r="Q7" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="Q7" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="R7" s="6"/>
       <c r="S7" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="T7" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="U7" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="V7" s="6">
         <v>100000</v>
@@ -1233,7 +1231,7 @@
         <v>120000</v>
       </c>
       <c r="Y7" s="6" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="Z7" s="6">
         <v>150000</v>
@@ -1241,64 +1239,65 @@
       <c r="AA7" s="6"/>
     </row>
     <row r="8" spans="1:27" s="10" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="8">
+      <c r="B8" s="14" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>XE_30922</v>
+      </c>
+      <c r="C8" s="13">
         <v>45575</v>
       </c>
       <c r="D8" s="8">
         <v>45576</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="F8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="7" t="s">
-        <v>27</v>
-      </c>
       <c r="H8" s="6" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="I8" s="6">
         <v>1500</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="K8" s="12">
         <v>100</v>
       </c>
       <c r="L8" s="6"/>
       <c r="M8" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="N8" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="N8" s="6" t="s">
+      <c r="O8" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="O8" s="7" t="s">
+      <c r="P8" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="P8" s="7" t="s">
+      <c r="Q8" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="Q8" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="R8" s="6"/>
       <c r="S8" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="T8" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="U8" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="V8" s="6">
         <v>100000</v>
@@ -1310,7 +1309,7 @@
         <v>120000</v>
       </c>
       <c r="Y8" s="6" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="Z8" s="6">
         <v>150000</v>

</xml_diff>

<commit_message>
Fix: Thêm bánh xe và giá khác
</commit_message>
<xml_diff>
--- a/src/main/resources/report_templates/EXCEL_TO_PRODUCTION_PRODUCT.xlsx
+++ b/src/main/resources/report_templates/EXCEL_TO_PRODUCTION_PRODUCT.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\MeuPro\MeUVipPro\src\main\resources\report_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MeU\MeuPro\MeUVipPro\src\main\resources\report_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D701D33-1F82-4725-BF99-5D224C5A6D97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6171A4E6-D924-43B5-A3E2-959E63BD6B89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="U3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="V3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -46,7 +46,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U4" authorId="0" shapeId="0" xr:uid="{500951B5-36AD-476A-924D-15E739ABB651}">
+    <comment ref="V4" authorId="0" shapeId="0" xr:uid="{500951B5-36AD-476A-924D-15E739ABB651}">
       <text>
         <r>
           <rPr>
@@ -62,7 +62,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U5" authorId="0" shapeId="0" xr:uid="{E702B8D1-3DAC-4CB1-9B52-E887B6E2ABDD}">
+    <comment ref="V5" authorId="0" shapeId="0" xr:uid="{E702B8D1-3DAC-4CB1-9B52-E887B6E2ABDD}">
       <text>
         <r>
           <rPr>
@@ -78,39 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U6" authorId="0" shapeId="0" xr:uid="{2FFB3B58-05CF-460D-AE7C-7651A5DB8135}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>======
-ID#AAABoy724XE
-Loan Hoang    (2025-08-05 08:43:04)
-Đã bị sửa và link với Cấu hình</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="U7" authorId="0" shapeId="0" xr:uid="{8108C992-B201-48D6-B77D-78C4150B4867}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>======
-ID#AAABoy724XE
-Loan Hoang    (2025-08-05 08:43:04)
-Đã bị sửa và link với Cấu hình</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="U8" authorId="0" shapeId="0" xr:uid="{31CA5816-2963-40B6-9C79-2A5210238A33}">
+    <comment ref="V6" authorId="0" shapeId="0" xr:uid="{2FFB3B58-05CF-460D-AE7C-7651A5DB8135}">
       <text>
         <r>
           <rPr>
@@ -136,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
   <si>
     <t>1. KHO HÀNG CHỜ SẢN XUẤT: Bao gồm các trường sau</t>
   </si>
@@ -235,6 +203,18 @@
   </si>
   <si>
     <t>XE</t>
+  </si>
+  <si>
+    <t>Bánh xe</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Giá khác</t>
+  </si>
+  <si>
+    <t>NV20241112</t>
   </si>
 </sst>
 </file>
@@ -673,10 +653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA999"/>
+  <dimension ref="A1:AC508"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T32" sqref="T32"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AC29" sqref="AC29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -699,17 +679,18 @@
     <col min="16" max="16" width="22.44140625" customWidth="1"/>
     <col min="17" max="17" width="15.109375" customWidth="1"/>
     <col min="18" max="19" width="8.6640625" customWidth="1"/>
-    <col min="20" max="20" width="75" customWidth="1"/>
-    <col min="21" max="21" width="18.5546875" customWidth="1"/>
-    <col min="22" max="22" width="19.109375" customWidth="1"/>
-    <col min="23" max="23" width="19.88671875" customWidth="1"/>
-    <col min="24" max="24" width="14.5546875" customWidth="1"/>
-    <col min="25" max="25" width="13.44140625" customWidth="1"/>
-    <col min="26" max="26" width="14.5546875" customWidth="1"/>
-    <col min="27" max="27" width="8.6640625" customWidth="1"/>
+    <col min="20" max="20" width="19.21875" customWidth="1"/>
+    <col min="21" max="21" width="75" customWidth="1"/>
+    <col min="22" max="22" width="18.5546875" customWidth="1"/>
+    <col min="23" max="23" width="19.109375" customWidth="1"/>
+    <col min="24" max="24" width="19.88671875" customWidth="1"/>
+    <col min="25" max="26" width="14.5546875" customWidth="1"/>
+    <col min="27" max="27" width="13.44140625" customWidth="1"/>
+    <col min="28" max="28" width="14.5546875" customWidth="1"/>
+    <col min="29" max="29" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -741,8 +722,10 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
       <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2"/>
     </row>
-    <row r="2" spans="1:27" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -801,37 +784,43 @@
         <v>17</v>
       </c>
       <c r="T2" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="U2" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="V2" s="20" t="s">
+      <c r="W2" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="W2" s="20" t="s">
+      <c r="X2" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="X2" s="20" t="s">
+      <c r="Y2" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="Y2" s="19" t="s">
+      <c r="Z2" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA2" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="Z2" s="19" t="s">
+      <c r="AB2" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AC2" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:27" s="9" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" s="9" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>24</v>
       </c>
       <c r="B3" s="13" t="str">
         <f ca="1">"XE_"&amp;TEXT(RANDBETWEEN(0,99999),"00000")</f>
-        <v>XE_58228</v>
+        <v>XE_71571</v>
       </c>
       <c r="C3" s="12">
         <v>45570</v>
@@ -843,7 +832,7 @@
         <v>32</v>
       </c>
       <c r="F3" s="8" t="str">
-        <f t="shared" ref="F3:F8" ca="1" si="0">"PPT_" &amp; RANDBETWEEN(1,5)</f>
+        <f t="shared" ref="F3:F7" ca="1" si="0">"PPT_" &amp; RANDBETWEEN(1,5)</f>
         <v>PPT_3</v>
       </c>
       <c r="G3" s="13" t="str">
@@ -852,15 +841,15 @@
 "FB25-12","FD30T-16",
 "J2.5XN","H3.0FT",
 "FE4P16","FE4P25","FE3D20N")</f>
-        <v>8FD25</v>
+        <v>H3.0FT</v>
       </c>
       <c r="H3" s="13" t="str">
         <f ca="1">"SN-" &amp; TEXT(TODAY(),"YYYYMM") &amp; "-" &amp; TEXT(RANDBETWEEN(1,99999),"00000")</f>
-        <v>SN-202509-53957</v>
+        <v>SN-202510-45359</v>
       </c>
       <c r="I3" s="13">
         <f ca="1">RANDBETWEEN(10,25)*100</f>
-        <v>2500</v>
+        <v>1700</v>
       </c>
       <c r="J3" s="13" t="str">
         <f ca="1">"KN" &amp; CHAR(RANDBETWEEN(65,70))</f>
@@ -868,7 +857,7 @@
       </c>
       <c r="K3" s="11">
         <f ca="1">RANDBETWEEN(30,60)*100</f>
-        <v>3400</v>
+        <v>3300</v>
       </c>
       <c r="L3" s="5" t="str">
         <f ca="1">CHOOSE(RANDBETWEEN(1,3),"AC","DC","AC 3Pha")</f>
@@ -876,7 +865,7 @@
       </c>
       <c r="M3" s="16" t="str">
         <f ca="1">CHOOSE(RANDBETWEEN(1,5),"Lithium-ion","Lead–Acid","Diesel","LPG","Gasoline")</f>
-        <v>Lithium-ion</v>
+        <v>LPG</v>
       </c>
       <c r="N3" s="13" t="str">
         <f ca="1">CHOOSE(RANDBETWEEN(1,2),"Lithium-ion","Lead–Acid")
@@ -886,15 +875,15 @@
 CHOOSE(RANDBETWEEN(1,3),240,360,480) &amp; "Ah"
  &amp; " | " &amp;
 RANDBETWEEN(200,600) &amp; " kg"</f>
-        <v>Lithium-ion | 48V | 480Ah | 333 kg</v>
+        <v>Lithium-ion | 24V | 360Ah | 585 kg</v>
       </c>
       <c r="O3" s="17" t="str">
         <f ca="1">RANDBETWEEN(1,50) &amp; "A"</f>
-        <v>25A</v>
+        <v>19A</v>
       </c>
       <c r="P3" s="6" t="str">
         <f ca="1">RANDBETWEEN(600,1200) &amp; " x " &amp; RANDBETWEEN(1000,1500) &amp; "mm"</f>
-        <v>784 x 1187mm</v>
+        <v>682 x 1257mm</v>
       </c>
       <c r="Q3" s="5" t="s">
         <v>25</v>
@@ -907,7 +896,10 @@
         <f ca="1">CHOOSE(RANDBETWEEN(1,2),"có","không")</f>
         <v>không</v>
       </c>
-      <c r="T3" s="8" t="str">
+      <c r="T3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="U3" s="8" t="str">
         <f ca="1">CHOOSE(RANDBETWEEN(1,2),"Lốp đặc","Lốp hơi") &amp; ", " &amp;
 ROUND(RAND()*(5-1)+1,1) &amp; "t, " &amp;
 ROUND(RAND()*(6-3)+3,1) &amp; "m, " &amp;
@@ -917,40 +909,44 @@
 RANDBETWEEN(1200,2500) &amp; " x " &amp; RANDBETWEEN(600,1500) &amp; "mm, " &amp;
 ROUND(RAND()*(20-5)+5,1) &amp; "km/h, " &amp;
 ROUND(RAND()*15,1) &amp; "°"</f>
-        <v>Lốp đặc, 1.3t, 3.6m, Diesel, Không, Trung bình, 1999 x 733mm, 10.9km/h, 9°</v>
-      </c>
-      <c r="U3" s="8" t="s">
+        <v>Lốp hơi, 1.1t, 5.1m, Điện, Không, Mới, 2342 x 789mm, 19.8km/h, 8.1°</v>
+      </c>
+      <c r="V3" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="V3" s="21">
+      <c r="W3" s="21">
         <f ca="1">RANDBETWEEN(1,5)*10</f>
-        <v>20</v>
-      </c>
-      <c r="W3" s="13">
+        <v>30</v>
+      </c>
+      <c r="X3" s="13">
         <f ca="1">RANDBETWEEN(16,20)*10</f>
-        <v>170</v>
-      </c>
-      <c r="X3" s="21">
+        <v>200</v>
+      </c>
+      <c r="Y3" s="21">
         <f ca="1">RANDBETWEEN(6,10)*10</f>
-        <v>100</v>
-      </c>
-      <c r="Y3" s="14" t="str">
+        <v>90</v>
+      </c>
+      <c r="Z3" s="21">
+        <f ca="1">RANDBETWEEN(6,10)*10</f>
+        <v>80</v>
+      </c>
+      <c r="AA3" s="14" t="str">
         <f ca="1">"Đại lý_" &amp; CHOOSE(RANDBETWEEN(1,5),"A","B","C","D","E")</f>
-        <v>Đại lý_D</v>
-      </c>
-      <c r="Z3" s="5">
+        <v>Đại lý_B</v>
+      </c>
+      <c r="AB3" s="5">
         <f ca="1">RANDBETWEEN(11,15)*10</f>
         <v>120</v>
       </c>
-      <c r="AA3" s="5"/>
+      <c r="AC3" s="5"/>
     </row>
-    <row r="4" spans="1:27" s="9" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" s="9" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="13" t="str">
-        <f t="shared" ref="B4:B8" ca="1" si="1">"XE_"&amp;TEXT(RANDBETWEEN(0,99999),"00000")</f>
-        <v>XE_19723</v>
+        <f t="shared" ref="B4:B5" ca="1" si="1">"XE_"&amp;TEXT(RANDBETWEEN(0,99999),"00000")</f>
+        <v>XE_43945</v>
       </c>
       <c r="C4" s="12">
         <v>45571</v>
@@ -963,7 +959,7 @@
       </c>
       <c r="F4" s="8" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>PPT_2</v>
+        <v>PPT_4</v>
       </c>
       <c r="G4" s="13" t="str">
         <f ca="1">CHOOSE(RANDBETWEEN(1,11),
@@ -974,60 +970,63 @@
         <v>8FD25</v>
       </c>
       <c r="H4" s="13" t="str">
-        <f t="shared" ref="H4:H8" ca="1" si="2">"SN-" &amp; TEXT(TODAY(),"YYYYMM") &amp; "-" &amp; TEXT(RANDBETWEEN(1,99999),"00000")</f>
-        <v>SN-202509-85916</v>
+        <f t="shared" ref="H4:H7" ca="1" si="2">"SN-" &amp; TEXT(TODAY(),"YYYYMM") &amp; "-" &amp; TEXT(RANDBETWEEN(1,99999),"00000")</f>
+        <v>SN-202510-50360</v>
       </c>
       <c r="I4" s="13">
-        <f t="shared" ref="I4:I8" ca="1" si="3">RANDBETWEEN(10,25)*100</f>
-        <v>2200</v>
+        <f t="shared" ref="I4:I7" ca="1" si="3">RANDBETWEEN(10,25)*100</f>
+        <v>2500</v>
       </c>
       <c r="J4" s="13" t="str">
-        <f t="shared" ref="J4:J8" ca="1" si="4">"KN" &amp; CHAR(RANDBETWEEN(65,70))</f>
-        <v>KNC</v>
+        <f t="shared" ref="J4:J7" ca="1" si="4">"KN" &amp; CHAR(RANDBETWEEN(65,70))</f>
+        <v>KNB</v>
       </c>
       <c r="K4" s="11">
-        <f t="shared" ref="K4:K8" ca="1" si="5">RANDBETWEEN(30,60)*100</f>
-        <v>5500</v>
+        <f t="shared" ref="K4:K7" ca="1" si="5">RANDBETWEEN(30,60)*100</f>
+        <v>3900</v>
       </c>
       <c r="L4" s="5" t="str">
-        <f t="shared" ref="L4:L8" ca="1" si="6">CHOOSE(RANDBETWEEN(1,3),"AC","DC","AC 3Pha")</f>
+        <f t="shared" ref="L4:L7" ca="1" si="6">CHOOSE(RANDBETWEEN(1,3),"AC","DC","AC 3Pha")</f>
         <v>DC</v>
       </c>
       <c r="M4" s="16" t="str">
-        <f t="shared" ref="M4:M8" ca="1" si="7">CHOOSE(RANDBETWEEN(1,5),"Lithium-ion","Lead–Acid","Diesel","LPG","Gasoline")</f>
-        <v>Gasoline</v>
+        <f t="shared" ref="M4:M7" ca="1" si="7">CHOOSE(RANDBETWEEN(1,5),"Lithium-ion","Lead–Acid","Diesel","LPG","Gasoline")</f>
+        <v>Diesel</v>
       </c>
       <c r="N4" s="13" t="str">
-        <f t="shared" ref="N4:N8" ca="1" si="8">CHOOSE(RANDBETWEEN(1,2),"Lithium-ion","Lead–Acid")
+        <f t="shared" ref="N4:N7" ca="1" si="8">CHOOSE(RANDBETWEEN(1,2),"Lithium-ion","Lead–Acid")
  &amp; " | " &amp;
 CHOOSE(RANDBETWEEN(1,4),24,36,48,72) &amp; "V"
  &amp; " | " &amp;
 CHOOSE(RANDBETWEEN(1,3),240,360,480) &amp; "Ah"
  &amp; " | " &amp;
 RANDBETWEEN(200,600) &amp; " kg"</f>
-        <v>Lithium-ion | 36V | 480Ah | 461 kg</v>
+        <v>Lithium-ion | 36V | 360Ah | 358 kg</v>
       </c>
       <c r="O4" s="17" t="str">
         <f t="shared" ref="O4:O7" ca="1" si="9">RANDBETWEEN(1,50) &amp; "A"</f>
-        <v>27A</v>
+        <v>20A</v>
       </c>
       <c r="P4" s="6" t="str">
-        <f t="shared" ref="P4:P8" ca="1" si="10">RANDBETWEEN(600,1200) &amp; " x " &amp; RANDBETWEEN(1000,1500) &amp; "mm"</f>
-        <v>644 x 1200mm</v>
+        <f t="shared" ref="P4:P7" ca="1" si="10">RANDBETWEEN(600,1200) &amp; " x " &amp; RANDBETWEEN(1000,1500) &amp; "mm"</f>
+        <v>969 x 1496mm</v>
       </c>
       <c r="Q4" s="5" t="s">
         <v>25</v>
       </c>
       <c r="R4" s="5">
-        <f t="shared" ref="R4:R8" ca="1" si="11">CHOOSE(RANDBETWEEN(1,3), 2, 3, 5)</f>
-        <v>5</v>
+        <f t="shared" ref="R4:R7" ca="1" si="11">CHOOSE(RANDBETWEEN(1,3), 2, 3, 5)</f>
+        <v>3</v>
       </c>
       <c r="S4" s="5" t="str">
-        <f t="shared" ref="S4:S8" ca="1" si="12">CHOOSE(RANDBETWEEN(1,2),"có","không")</f>
+        <f t="shared" ref="S4:S7" ca="1" si="12">CHOOSE(RANDBETWEEN(1,2),"có","không")</f>
         <v>có</v>
       </c>
-      <c r="T4" s="8" t="str">
-        <f t="shared" ref="T4:T8" ca="1" si="13">CHOOSE(RANDBETWEEN(1,2),"Lốp đặc","Lốp hơi") &amp; ", " &amp;
+      <c r="T4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="U4" s="8" t="str">
+        <f t="shared" ref="U4:U7" ca="1" si="13">CHOOSE(RANDBETWEEN(1,2),"Lốp đặc","Lốp hơi") &amp; ", " &amp;
 ROUND(RAND()*(5-1)+1,1) &amp; "t, " &amp;
 ROUND(RAND()*(6-3)+3,1) &amp; "m, " &amp;
 CHOOSE(RANDBETWEEN(1,3),"Điện","Diesel","Gas") &amp; ", " &amp;
@@ -1036,40 +1035,44 @@
 RANDBETWEEN(1200,2500) &amp; " x " &amp; RANDBETWEEN(600,1500) &amp; "mm, " &amp;
 ROUND(RAND()*(20-5)+5,1) &amp; "km/h, " &amp;
 ROUND(RAND()*15,1) &amp; "°"</f>
-        <v>Lốp đặc, 3.8t, 3.5m, Điện, Không, Cũ, 2428 x 1134mm, 9.4km/h, 5.2°</v>
-      </c>
-      <c r="U4" s="8" t="s">
+        <v>Lốp đặc, 3.5t, 3.7m, Điện, Không, Trung bình, 2070 x 1369mm, 16.2km/h, 10.4°</v>
+      </c>
+      <c r="V4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="V4" s="21">
-        <f t="shared" ref="V4:V8" ca="1" si="14">RANDBETWEEN(1,5)*10</f>
-        <v>50</v>
-      </c>
-      <c r="W4" s="13">
-        <f t="shared" ref="W4:W8" ca="1" si="15">RANDBETWEEN(16,20)*10</f>
-        <v>190</v>
-      </c>
-      <c r="X4" s="21">
-        <f t="shared" ref="X4:X8" ca="1" si="16">RANDBETWEEN(6,10)*10</f>
+      <c r="W4" s="21">
+        <f t="shared" ref="W4:W7" ca="1" si="14">RANDBETWEEN(1,5)*10</f>
+        <v>10</v>
+      </c>
+      <c r="X4" s="13">
+        <f t="shared" ref="X4:X7" ca="1" si="15">RANDBETWEEN(16,20)*10</f>
+        <v>200</v>
+      </c>
+      <c r="Y4" s="21">
+        <f t="shared" ref="Y4:Z7" ca="1" si="16">RANDBETWEEN(6,10)*10</f>
         <v>90</v>
       </c>
-      <c r="Y4" s="14" t="str">
-        <f t="shared" ref="Y4:Y8" ca="1" si="17">"Đại lý_" &amp; CHOOSE(RANDBETWEEN(1,5),"A","B","C","D","E")</f>
+      <c r="Z4" s="21">
+        <f t="shared" ca="1" si="16"/>
+        <v>60</v>
+      </c>
+      <c r="AA4" s="14" t="str">
+        <f t="shared" ref="AA4:AA7" ca="1" si="17">"Đại lý_" &amp; CHOOSE(RANDBETWEEN(1,5),"A","B","C","D","E")</f>
         <v>Đại lý_E</v>
       </c>
-      <c r="Z4" s="5">
-        <f t="shared" ref="Z4:Z8" ca="1" si="18">RANDBETWEEN(11,15)*10</f>
-        <v>120</v>
-      </c>
-      <c r="AA4" s="5"/>
+      <c r="AB4" s="5">
+        <f t="shared" ref="AB4:AB7" ca="1" si="18">RANDBETWEEN(11,15)*10</f>
+        <v>150</v>
+      </c>
+      <c r="AC4" s="5"/>
     </row>
-    <row r="5" spans="1:27" s="9" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" s="9" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="13" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>XE_78460</v>
+        <v>XE_09439</v>
       </c>
       <c r="C5" s="12">
         <v>45572</v>
@@ -1082,35 +1085,35 @@
       </c>
       <c r="F5" s="8" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>PPT_1</v>
+        <v>PPT_2</v>
       </c>
       <c r="G5" s="13" t="str">
-        <f t="shared" ref="G4:G8" ca="1" si="19">CHOOSE(RANDBETWEEN(1,11),
+        <f t="shared" ref="G5:G7" ca="1" si="19">CHOOSE(RANDBETWEEN(1,11),
 "8FB15","8FD25","7FBEU18",
 "FB25-12","FD30T-16",
 "J2.5XN","H3.0FT",
 "FE4P16","FE4P25","FE3D20N")</f>
-        <v>FE3D20N</v>
+        <v>7FBEU18</v>
       </c>
       <c r="H5" s="13" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>SN-202509-75826</v>
+        <v>SN-202510-58082</v>
       </c>
       <c r="I5" s="13">
         <f t="shared" ca="1" si="3"/>
-        <v>1700</v>
+        <v>2200</v>
       </c>
       <c r="J5" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>KNA</v>
+        <v>KNF</v>
       </c>
       <c r="K5" s="11">
         <f t="shared" ca="1" si="5"/>
-        <v>4300</v>
+        <v>5400</v>
       </c>
       <c r="L5" s="5" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>DC</v>
+        <v>AC</v>
       </c>
       <c r="M5" s="16" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -1118,63 +1121,70 @@
       </c>
       <c r="N5" s="13" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>Lithium-ion | 36V | 240Ah | 408 kg</v>
+        <v>Lithium-ion | 36V | 240Ah | 549 kg</v>
       </c>
       <c r="O5" s="17" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>45A</v>
+        <v>14A</v>
       </c>
       <c r="P5" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>1100 x 1405mm</v>
+        <v>746 x 1179mm</v>
       </c>
       <c r="Q5" s="5" t="s">
         <v>25</v>
       </c>
       <c r="R5" s="5">
         <f t="shared" ca="1" si="11"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S5" s="5" t="str">
         <f t="shared" ca="1" si="12"/>
         <v>có</v>
       </c>
-      <c r="T5" s="8" t="str">
+      <c r="T5" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="U5" s="8" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>Lốp hơi, 1.5t, 3.1m, Diesel, Không, Mới, 1300 x 1310mm, 9.7km/h, 4.1°</v>
-      </c>
-      <c r="U5" s="8" t="s">
+        <v>Lốp hơi, 1.9t, 3.2m, Gas, Có, Cũ, 1961 x 1353mm, 11.8km/h, 6.8°</v>
+      </c>
+      <c r="V5" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="V5" s="21">
+      <c r="W5" s="21">
         <f t="shared" ca="1" si="14"/>
-        <v>50</v>
-      </c>
-      <c r="W5" s="13">
+        <v>20</v>
+      </c>
+      <c r="X5" s="13">
         <f t="shared" ca="1" si="15"/>
-        <v>180</v>
-      </c>
-      <c r="X5" s="21">
+        <v>170</v>
+      </c>
+      <c r="Y5" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>70</v>
-      </c>
-      <c r="Y5" s="14" t="str">
+        <v>60</v>
+      </c>
+      <c r="Z5" s="21">
+        <f t="shared" ca="1" si="16"/>
+        <v>90</v>
+      </c>
+      <c r="AA5" s="14" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>Đại lý_C</v>
-      </c>
-      <c r="Z5" s="5">
+        <v>Đại lý_A</v>
+      </c>
+      <c r="AB5" s="5">
         <f t="shared" ca="1" si="18"/>
         <v>110</v>
       </c>
-      <c r="AA5" s="5"/>
+      <c r="AC5" s="5"/>
     </row>
-    <row r="6" spans="1:27" s="9" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" s="9" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>24</v>
       </c>
       <c r="B6" s="13" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>XE_14527</v>
+        <f ca="1">"XE_"&amp;TEXT(RANDBETWEEN(0,99999),"00000")</f>
+        <v>XE_93128</v>
       </c>
       <c r="C6" s="12">
         <v>45573</v>
@@ -1187,39 +1197,39 @@
       </c>
       <c r="F6" s="8" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>PPT_2</v>
+        <v>PPT_3</v>
       </c>
       <c r="G6" s="13" t="str">
         <f t="shared" ca="1" si="19"/>
-        <v>FE4P16</v>
+        <v>H3.0FT</v>
       </c>
       <c r="H6" s="13" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>SN-202509-65678</v>
+        <v>SN-202510-62801</v>
       </c>
       <c r="I6" s="13">
         <f t="shared" ca="1" si="3"/>
-        <v>2000</v>
+        <v>1600</v>
       </c>
       <c r="J6" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>KNA</v>
+        <v>KND</v>
       </c>
       <c r="K6" s="11">
         <f t="shared" ca="1" si="5"/>
-        <v>4500</v>
+        <v>6000</v>
       </c>
       <c r="L6" s="5" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>AC 3Pha</v>
+        <v>AC</v>
       </c>
       <c r="M6" s="16" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>Gasoline</v>
+        <v>Lead–Acid</v>
       </c>
       <c r="N6" s="13" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>Lead–Acid | 72V | 360Ah | 392 kg</v>
+        <v>Lithium-ion | 48V | 240Ah | 574 kg</v>
       </c>
       <c r="O6" s="17" t="str">
         <f t="shared" ca="1" si="9"/>
@@ -1227,7 +1237,7 @@
       </c>
       <c r="P6" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>625 x 1190mm</v>
+        <v>1072 x 1484mm</v>
       </c>
       <c r="Q6" s="5" t="s">
         <v>25</v>
@@ -1240,45 +1250,52 @@
         <f t="shared" ca="1" si="12"/>
         <v>không</v>
       </c>
-      <c r="T6" s="8" t="str">
+      <c r="T6" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="U6" s="8" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>Lốp đặc, 2t, 5.6m, Diesel, Có, Cũ, 2329 x 873mm, 17.3km/h, 2.1°</v>
-      </c>
-      <c r="U6" s="8" t="s">
+        <v>Lốp hơi, 2.5t, 3.7m, Gas, Có, Mới, 2165 x 1152mm, 7.9km/h, 3.8°</v>
+      </c>
+      <c r="V6" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="V6" s="21">
+      <c r="W6" s="21">
         <f t="shared" ca="1" si="14"/>
-        <v>30</v>
-      </c>
-      <c r="W6" s="13">
+        <v>10</v>
+      </c>
+      <c r="X6" s="13">
         <f t="shared" ca="1" si="15"/>
-        <v>170</v>
-      </c>
-      <c r="X6" s="21">
+        <v>160</v>
+      </c>
+      <c r="Y6" s="21">
+        <f t="shared" ca="1" si="16"/>
+        <v>60</v>
+      </c>
+      <c r="Z6" s="21">
         <f t="shared" ca="1" si="16"/>
         <v>100</v>
       </c>
-      <c r="Y6" s="14" t="str">
+      <c r="AA6" s="14" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>Đại lý_D</v>
-      </c>
-      <c r="Z6" s="5">
+        <v>Đại lý_E</v>
+      </c>
+      <c r="AB6" s="5">
         <f t="shared" ca="1" si="18"/>
-        <v>140</v>
-      </c>
-      <c r="AA6" s="5"/>
+        <v>120</v>
+      </c>
+      <c r="AC6" s="5"/>
     </row>
-    <row r="7" spans="1:27" s="9" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29" s="9" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="B7" s="13" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>XE_83875</v>
+        <f ca="1">"XE_"&amp;TEXT(RANDBETWEEN(0,99999),"00000")</f>
+        <v>XE_31056</v>
       </c>
       <c r="C7" s="12">
-        <v>45574</v>
+        <v>45573</v>
       </c>
       <c r="D7" s="7">
         <v>45576</v>
@@ -1290,21 +1307,17 @@
         <f t="shared" ca="1" si="0"/>
         <v>PPT_4</v>
       </c>
-      <c r="G7" s="13" t="str">
-        <f ca="1">CHOOSE(RANDBETWEEN(1,11),
-"8FB15","8FD25","7FBEU18",
-"FB25-12","FD30T-16",
-"J2.5XN","H3.0FT",
-"FE4P16","FE4P25","FE3D20N")</f>
-        <v>FE4P16</v>
+      <c r="G7" s="13" t="e">
+        <f t="shared" ca="1" si="19"/>
+        <v>#VALUE!</v>
       </c>
       <c r="H7" s="13" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>SN-202509-88209</v>
+        <v>SN-202510-83707</v>
       </c>
       <c r="I7" s="13">
         <f t="shared" ca="1" si="3"/>
-        <v>1000</v>
+        <v>2500</v>
       </c>
       <c r="J7" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -1312,27 +1325,27 @@
       </c>
       <c r="K7" s="11">
         <f t="shared" ca="1" si="5"/>
-        <v>6000</v>
+        <v>3500</v>
       </c>
       <c r="L7" s="5" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>AC 3Pha</v>
+        <v>DC</v>
       </c>
       <c r="M7" s="16" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>Diesel</v>
+        <v>Lithium-ion</v>
       </c>
       <c r="N7" s="13" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>Lead–Acid | 24V | 240Ah | 597 kg</v>
+        <v>Lithium-ion | 72V | 240Ah | 559 kg</v>
       </c>
       <c r="O7" s="17" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>37A</v>
+        <v>45A</v>
       </c>
       <c r="P7" s="6" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>1034 x 1015mm</v>
+        <v>878 x 1492mm</v>
       </c>
       <c r="Q7" s="5" t="s">
         <v>25</v>
@@ -1343,146 +1356,53 @@
       </c>
       <c r="S7" s="5" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>không</v>
-      </c>
-      <c r="T7" s="8" t="str">
+        <v>có</v>
+      </c>
+      <c r="T7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="U7" s="8" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>Lốp hơi, 3.5t, 3.1m, Gas, Có, Mới, 1265 x 866mm, 13.6km/h, 6°</v>
-      </c>
-      <c r="U7" s="8" t="s">
+        <v>Lốp hơi, 4.8t, 4.3m, Gas, Không, Mới, 2489 x 877mm, 8.2km/h, 10.3°</v>
+      </c>
+      <c r="V7" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="V7" s="21">
+      <c r="W7" s="21">
         <f t="shared" ca="1" si="14"/>
-        <v>40</v>
-      </c>
-      <c r="W7" s="13">
+        <v>50</v>
+      </c>
+      <c r="X7" s="13">
         <f t="shared" ca="1" si="15"/>
         <v>200</v>
       </c>
-      <c r="X7" s="21">
-        <f t="shared" ca="1" si="16"/>
-        <v>100</v>
-      </c>
-      <c r="Y7" s="14" t="str">
-        <f t="shared" ca="1" si="17"/>
-        <v>Đại lý_B</v>
-      </c>
-      <c r="Z7" s="5">
-        <f t="shared" ca="1" si="18"/>
-        <v>130</v>
-      </c>
-      <c r="AA7" s="5"/>
-    </row>
-    <row r="8" spans="1:27" s="9" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="13" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>XE_01309</v>
-      </c>
-      <c r="C8" s="12">
-        <v>45575</v>
-      </c>
-      <c r="D8" s="7">
-        <v>45576</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>PPT_4</v>
-      </c>
-      <c r="G8" s="13" t="str">
-        <f t="shared" ca="1" si="19"/>
-        <v>8FB15</v>
-      </c>
-      <c r="H8" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>SN-202509-84724</v>
-      </c>
-      <c r="I8" s="13">
-        <f t="shared" ca="1" si="3"/>
-        <v>1900</v>
-      </c>
-      <c r="J8" s="13" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>KNB</v>
-      </c>
-      <c r="K8" s="11">
-        <f t="shared" ca="1" si="5"/>
-        <v>6000</v>
-      </c>
-      <c r="L8" s="5" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v>AC 3Pha</v>
-      </c>
-      <c r="M8" s="16" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>Lead–Acid</v>
-      </c>
-      <c r="N8" s="13" t="str">
-        <f t="shared" ca="1" si="8"/>
-        <v>Lead–Acid | 48V | 480Ah | 485 kg</v>
-      </c>
-      <c r="O8" s="17" t="str">
-        <f ca="1">RANDBETWEEN(1,50) &amp; "A"</f>
-        <v>11A</v>
-      </c>
-      <c r="P8" s="6" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>933 x 1207mm</v>
-      </c>
-      <c r="Q8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="R8" s="5">
-        <f t="shared" ca="1" si="11"/>
-        <v>2</v>
-      </c>
-      <c r="S8" s="5" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>có</v>
-      </c>
-      <c r="T8" s="8" t="str">
-        <f t="shared" ca="1" si="13"/>
-        <v>Lốp đặc, 4.6t, 3.2m, Diesel, Không, Trung bình, 2389 x 713mm, 16.9km/h, 5.1°</v>
-      </c>
-      <c r="U8" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="V8" s="21">
-        <f t="shared" ca="1" si="14"/>
-        <v>40</v>
-      </c>
-      <c r="W8" s="13">
-        <f t="shared" ca="1" si="15"/>
-        <v>170</v>
-      </c>
-      <c r="X8" s="21">
+      <c r="Y7" s="21">
         <f t="shared" ca="1" si="16"/>
         <v>80</v>
       </c>
-      <c r="Y8" s="14" t="str">
+      <c r="Z7" s="21">
+        <f t="shared" ca="1" si="16"/>
+        <v>60</v>
+      </c>
+      <c r="AA7" s="14" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>Đại lý_D</v>
-      </c>
-      <c r="Z8" s="5">
+        <v>Đại lý_C</v>
+      </c>
+      <c r="AB7" s="5">
         <f t="shared" ca="1" si="18"/>
         <v>150</v>
       </c>
-      <c r="AA8" s="5"/>
+      <c r="AC7" s="5"/>
     </row>
-    <row r="9" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:29" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:29" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:29" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:29" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:29" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:29" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:29" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:29" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:29" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="17" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="18" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="19" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1975,501 +1895,10 @@
     <row r="506" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="507" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="508" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="509" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="510" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="511" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="512" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="513" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="514" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="515" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="516" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="517" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="518" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="519" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="520" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="521" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="522" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="523" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="524" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="525" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="526" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="527" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="528" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="529" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="530" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="531" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="532" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="533" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="534" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="535" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="536" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="537" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="538" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="539" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="540" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="541" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="542" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="543" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="544" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="545" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="546" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="547" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="548" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="549" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="550" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="551" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="552" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="553" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="554" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="555" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="556" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="557" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="558" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="559" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="560" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="561" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="562" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="563" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="564" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="565" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="566" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="567" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="568" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="569" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="570" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="571" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="572" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="573" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="574" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="575" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="576" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="577" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="578" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="579" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="580" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="581" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="582" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="583" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="584" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="585" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="586" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="587" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="588" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="589" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="590" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="591" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="592" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="593" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="594" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="595" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="596" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="597" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="598" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="599" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="600" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="601" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="602" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="603" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="604" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="605" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="606" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="607" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="608" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="609" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="610" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="611" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="612" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="613" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="614" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="615" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="616" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="617" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="618" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="619" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="620" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="621" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="622" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="623" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="624" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="625" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="626" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="627" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="628" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="629" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="630" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="631" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="632" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="633" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="634" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="635" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="636" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="637" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="638" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="639" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="640" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="641" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="642" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="643" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="644" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="645" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="646" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="647" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="648" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="649" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="650" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="651" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="652" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="653" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="654" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="655" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="656" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="657" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="658" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="659" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="660" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="661" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="662" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="663" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="664" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="665" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="666" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="667" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="668" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="669" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="670" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="671" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="672" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="673" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="674" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="675" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="676" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="677" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="678" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="679" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="680" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="681" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="682" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="683" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="684" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="685" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="686" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="687" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="688" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="689" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="690" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="691" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="692" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="693" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="694" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="695" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="696" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="697" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="698" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="699" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="700" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="701" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="702" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="703" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="704" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="705" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="706" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="707" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="708" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="709" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="710" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="711" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="712" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="713" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="714" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="715" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="716" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="717" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="718" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="719" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="720" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="721" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="722" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="723" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="724" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="725" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="726" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="727" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="728" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="729" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="730" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="731" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="732" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="733" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="734" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="735" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="736" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="737" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="738" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="739" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="740" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="741" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="742" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="743" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="744" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="745" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="746" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="747" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="748" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="749" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="750" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="751" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="752" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="753" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="754" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="755" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="756" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="757" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="758" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="759" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="760" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="761" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="762" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="763" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="764" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="765" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="766" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="767" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="768" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="769" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="770" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="771" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="772" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="773" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="774" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="775" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="776" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="777" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="778" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="779" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="780" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="781" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="782" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="783" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="784" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="785" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="786" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="787" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="788" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="789" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="790" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="791" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="792" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="793" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="794" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="795" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="796" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="797" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="798" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="799" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="800" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="801" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="802" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="803" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="804" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="805" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="806" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="807" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="808" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="809" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="810" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="811" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="812" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="813" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="814" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="815" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="816" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="817" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="818" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="819" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="820" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="821" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="822" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="823" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="824" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="825" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="826" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="827" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="828" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="829" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="830" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="831" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="832" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="833" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="834" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="835" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="836" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="837" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="838" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="839" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="840" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="841" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="842" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="843" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="844" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="845" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="846" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="847" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="848" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="849" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="850" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="851" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="852" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="853" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="854" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="855" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="856" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="857" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="858" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="859" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="860" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="861" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="862" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="863" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="864" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="865" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="866" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="867" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="868" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="869" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="870" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="871" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="872" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="873" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="874" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="875" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="876" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="877" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="878" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="879" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="880" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="881" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="882" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="883" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="884" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="885" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="886" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="887" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="888" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="889" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="890" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="891" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="892" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="893" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="894" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="895" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="896" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="897" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="898" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="899" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="900" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="901" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="902" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="903" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="904" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="905" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="906" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="907" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="908" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="909" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="910" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="911" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="912" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="913" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="914" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="915" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="916" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="917" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="918" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="919" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="920" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="921" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="922" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="923" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="924" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="925" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="926" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="927" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="928" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="929" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="930" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="931" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="932" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="933" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="934" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="935" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="936" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="937" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="938" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="939" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="940" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="941" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="942" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="943" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="944" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="945" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="946" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="947" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="948" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="949" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="950" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="951" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="952" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="953" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="954" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="955" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="956" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="957" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="958" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="959" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="960" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="961" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="962" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="963" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="964" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="965" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="966" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="967" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="968" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="969" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="970" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="971" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="972" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="973" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="974" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="975" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="976" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="977" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="978" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="979" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="980" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="981" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="982" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="983" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="984" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="985" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="986" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="987" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="988" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="989" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="990" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="991" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="992" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="993" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="994" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="995" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="996" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="997" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="998" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="999" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix: bổ sung detail trả về khi import
</commit_message>
<xml_diff>
--- a/src/main/resources/report_templates/EXCEL_TO_PRODUCTION_PRODUCT.xlsx
+++ b/src/main/resources/report_templates/EXCEL_TO_PRODUCTION_PRODUCT.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MeU\MeuPro\MeUVipPro\src\main\resources\report_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6171A4E6-D924-43B5-A3E2-959E63BD6B89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73F56760-9808-4878-9D0A-055AF060BA98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,6 +37,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -53,6 +54,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -69,6 +71,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -85,6 +88,7 @@
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>======
@@ -104,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="90">
   <si>
     <t>1. KHO HÀNG CHỜ SẢN XUẤT: Bao gồm các trường sau</t>
   </si>
@@ -215,13 +219,172 @@
   </si>
   <si>
     <t>NV20241112</t>
+  </si>
+  <si>
+    <t>XE_71571</t>
+  </si>
+  <si>
+    <t>PPT_3</t>
+  </si>
+  <si>
+    <t>H3.0FT</t>
+  </si>
+  <si>
+    <t>SN-202510-45359</t>
+  </si>
+  <si>
+    <t>KNA</t>
+  </si>
+  <si>
+    <t>DC</t>
+  </si>
+  <si>
+    <t>LPG</t>
+  </si>
+  <si>
+    <t>Lithium-ion | 24V | 360Ah | 585 kg</t>
+  </si>
+  <si>
+    <t>19A</t>
+  </si>
+  <si>
+    <t>682 x 1257mm</t>
+  </si>
+  <si>
+    <t>không</t>
+  </si>
+  <si>
+    <t>Lốp hơi, 1.1t, 5.1m, Điện, Không, Mới, 2342 x 789mm, 19.8km/h, 8.1°</t>
+  </si>
+  <si>
+    <t>Đại lý_B</t>
+  </si>
+  <si>
+    <t>XE_43945</t>
+  </si>
+  <si>
+    <t>PPT_4</t>
+  </si>
+  <si>
+    <t>8FD25</t>
+  </si>
+  <si>
+    <t>SN-202510-50360</t>
+  </si>
+  <si>
+    <t>KNB</t>
+  </si>
+  <si>
+    <t>Diesel</t>
+  </si>
+  <si>
+    <t>Lithium-ion | 36V | 360Ah | 358 kg</t>
+  </si>
+  <si>
+    <t>20A</t>
+  </si>
+  <si>
+    <t>969 x 1496mm</t>
+  </si>
+  <si>
+    <t>có</t>
+  </si>
+  <si>
+    <t>Lốp đặc, 3.5t, 3.7m, Điện, Không, Trung bình, 2070 x 1369mm, 16.2km/h, 10.4°</t>
+  </si>
+  <si>
+    <t>Đại lý_E</t>
+  </si>
+  <si>
+    <t>XE_09439</t>
+  </si>
+  <si>
+    <t>PPT_2</t>
+  </si>
+  <si>
+    <t>7FBEU18</t>
+  </si>
+  <si>
+    <t>SN-202510-58082</t>
+  </si>
+  <si>
+    <t>KNF</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>Lead–Acid</t>
+  </si>
+  <si>
+    <t>Lithium-ion | 36V | 240Ah | 549 kg</t>
+  </si>
+  <si>
+    <t>14A</t>
+  </si>
+  <si>
+    <t>746 x 1179mm</t>
+  </si>
+  <si>
+    <t>Lốp hơi, 1.9t, 3.2m, Gas, Có, Cũ, 1961 x 1353mm, 11.8km/h, 6.8°</t>
+  </si>
+  <si>
+    <t>Đại lý_A</t>
+  </si>
+  <si>
+    <t>XE_93128</t>
+  </si>
+  <si>
+    <t>KND</t>
+  </si>
+  <si>
+    <t>Lithium-ion | 48V | 240Ah | 574 kg</t>
+  </si>
+  <si>
+    <t>8A</t>
+  </si>
+  <si>
+    <t>1072 x 1484mm</t>
+  </si>
+  <si>
+    <t>Lốp hơi, 2.5t, 3.7m, Gas, Có, Mới, 2165 x 1152mm, 7.9km/h, 3.8°</t>
+  </si>
+  <si>
+    <t>XE_31056</t>
+  </si>
+  <si>
+    <t>SN-202510-83707</t>
+  </si>
+  <si>
+    <t>Lithium-ion</t>
+  </si>
+  <si>
+    <t>Lithium-ion | 72V | 240Ah | 559 kg</t>
+  </si>
+  <si>
+    <t>45A</t>
+  </si>
+  <si>
+    <t>878 x 1492mm</t>
+  </si>
+  <si>
+    <t>Lốp hơi, 4.8t, 4.3m, Gas, Không, Mới, 2489 x 877mm, 8.2km/h, 10.3°</t>
+  </si>
+  <si>
+    <t>Đại lý_C</t>
+  </si>
+  <si>
+    <t>SN-202510-58083</t>
+  </si>
+  <si>
+    <t>93.0AT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,21 +392,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -255,6 +428,7 @@
     <font>
       <sz val="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -379,65 +553,66 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -655,8 +830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC508"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AC29" sqref="AC29"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -818,9 +993,8 @@
       <c r="A3" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="13" t="str">
-        <f ca="1">"XE_"&amp;TEXT(RANDBETWEEN(0,99999),"00000")</f>
-        <v>XE_71571</v>
+      <c r="B3" s="13" t="s">
+        <v>37</v>
       </c>
       <c r="C3" s="12">
         <v>45570</v>
@@ -831,111 +1005,73 @@
       <c r="E3" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="8" t="str">
-        <f t="shared" ref="F3:F7" ca="1" si="0">"PPT_" &amp; RANDBETWEEN(1,5)</f>
-        <v>PPT_3</v>
-      </c>
-      <c r="G3" s="13" t="str">
-        <f ca="1">CHOOSE(RANDBETWEEN(1,11),
-"8FB15","8FD25","7FBEU18",
-"FB25-12","FD30T-16",
-"J2.5XN","H3.0FT",
-"FE4P16","FE4P25","FE3D20N")</f>
-        <v>H3.0FT</v>
-      </c>
-      <c r="H3" s="13" t="str">
-        <f ca="1">"SN-" &amp; TEXT(TODAY(),"YYYYMM") &amp; "-" &amp; TEXT(RANDBETWEEN(1,99999),"00000")</f>
-        <v>SN-202510-45359</v>
+      <c r="F3" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>40</v>
       </c>
       <c r="I3" s="13">
-        <f ca="1">RANDBETWEEN(10,25)*100</f>
         <v>1700</v>
       </c>
-      <c r="J3" s="13" t="str">
-        <f ca="1">"KN" &amp; CHAR(RANDBETWEEN(65,70))</f>
-        <v>KNA</v>
+      <c r="J3" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="K3" s="11">
-        <f ca="1">RANDBETWEEN(30,60)*100</f>
         <v>3300</v>
       </c>
-      <c r="L3" s="5" t="str">
-        <f ca="1">CHOOSE(RANDBETWEEN(1,3),"AC","DC","AC 3Pha")</f>
-        <v>DC</v>
-      </c>
-      <c r="M3" s="16" t="str">
-        <f ca="1">CHOOSE(RANDBETWEEN(1,5),"Lithium-ion","Lead–Acid","Diesel","LPG","Gasoline")</f>
-        <v>LPG</v>
-      </c>
-      <c r="N3" s="13" t="str">
-        <f ca="1">CHOOSE(RANDBETWEEN(1,2),"Lithium-ion","Lead–Acid")
- &amp; " | " &amp;
-CHOOSE(RANDBETWEEN(1,4),24,36,48,72) &amp; "V"
- &amp; " | " &amp;
-CHOOSE(RANDBETWEEN(1,3),240,360,480) &amp; "Ah"
- &amp; " | " &amp;
-RANDBETWEEN(200,600) &amp; " kg"</f>
-        <v>Lithium-ion | 24V | 360Ah | 585 kg</v>
-      </c>
-      <c r="O3" s="17" t="str">
-        <f ca="1">RANDBETWEEN(1,50) &amp; "A"</f>
-        <v>19A</v>
-      </c>
-      <c r="P3" s="6" t="str">
-        <f ca="1">RANDBETWEEN(600,1200) &amp; " x " &amp; RANDBETWEEN(1000,1500) &amp; "mm"</f>
-        <v>682 x 1257mm</v>
+      <c r="L3" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="M3" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="N3" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="O3" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>46</v>
       </c>
       <c r="Q3" s="5" t="s">
         <v>25</v>
       </c>
       <c r="R3" s="5">
-        <f ca="1">CHOOSE(RANDBETWEEN(1,3), 2, 3, 5)</f>
         <v>2</v>
       </c>
-      <c r="S3" s="5" t="str">
-        <f ca="1">CHOOSE(RANDBETWEEN(1,2),"có","không")</f>
-        <v>không</v>
+      <c r="S3" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="T3" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="U3" s="8" t="str">
-        <f ca="1">CHOOSE(RANDBETWEEN(1,2),"Lốp đặc","Lốp hơi") &amp; ", " &amp;
-ROUND(RAND()*(5-1)+1,1) &amp; "t, " &amp;
-ROUND(RAND()*(6-3)+3,1) &amp; "m, " &amp;
-CHOOSE(RANDBETWEEN(1,3),"Điện","Diesel","Gas") &amp; ", " &amp;
-CHOOSE(RANDBETWEEN(1,2),"Có","Không") &amp; ", " &amp;
-CHOOSE(RANDBETWEEN(1,3),"Mới","Trung bình","Cũ") &amp; ", " &amp;
-RANDBETWEEN(1200,2500) &amp; " x " &amp; RANDBETWEEN(600,1500) &amp; "mm, " &amp;
-ROUND(RAND()*(20-5)+5,1) &amp; "km/h, " &amp;
-ROUND(RAND()*15,1) &amp; "°"</f>
-        <v>Lốp hơi, 1.1t, 5.1m, Điện, Không, Mới, 2342 x 789mm, 19.8km/h, 8.1°</v>
+      <c r="U3" s="8" t="s">
+        <v>48</v>
       </c>
       <c r="V3" s="8" t="s">
         <v>26</v>
       </c>
       <c r="W3" s="21">
-        <f ca="1">RANDBETWEEN(1,5)*10</f>
         <v>30</v>
       </c>
       <c r="X3" s="13">
-        <f ca="1">RANDBETWEEN(16,20)*10</f>
         <v>200</v>
       </c>
       <c r="Y3" s="21">
-        <f ca="1">RANDBETWEEN(6,10)*10</f>
         <v>90</v>
       </c>
       <c r="Z3" s="21">
-        <f ca="1">RANDBETWEEN(6,10)*10</f>
         <v>80</v>
       </c>
-      <c r="AA3" s="14" t="str">
-        <f ca="1">"Đại lý_" &amp; CHOOSE(RANDBETWEEN(1,5),"A","B","C","D","E")</f>
-        <v>Đại lý_B</v>
+      <c r="AA3" s="14" t="s">
+        <v>49</v>
       </c>
       <c r="AB3" s="5">
-        <f ca="1">RANDBETWEEN(11,15)*10</f>
         <v>120</v>
       </c>
       <c r="AC3" s="5"/>
@@ -944,9 +1080,8 @@
       <c r="A4" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="13" t="str">
-        <f t="shared" ref="B4:B5" ca="1" si="1">"XE_"&amp;TEXT(RANDBETWEEN(0,99999),"00000")</f>
-        <v>XE_43945</v>
+      <c r="B4" s="13" t="s">
+        <v>50</v>
       </c>
       <c r="C4" s="12">
         <v>45571</v>
@@ -957,111 +1092,73 @@
       <c r="E4" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>PPT_4</v>
-      </c>
-      <c r="G4" s="13" t="str">
-        <f ca="1">CHOOSE(RANDBETWEEN(1,11),
-"8FB15","8FD25","7FBEU18",
-"FB25-12","FD30T-16",
-"J2.5XN","H3.0FT",
-"FE4P16","FE4P25","FE3D20N")</f>
-        <v>8FD25</v>
-      </c>
-      <c r="H4" s="13" t="str">
-        <f t="shared" ref="H4:H7" ca="1" si="2">"SN-" &amp; TEXT(TODAY(),"YYYYMM") &amp; "-" &amp; TEXT(RANDBETWEEN(1,99999),"00000")</f>
-        <v>SN-202510-50360</v>
+      <c r="F4" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>53</v>
       </c>
       <c r="I4" s="13">
-        <f t="shared" ref="I4:I7" ca="1" si="3">RANDBETWEEN(10,25)*100</f>
         <v>2500</v>
       </c>
-      <c r="J4" s="13" t="str">
-        <f t="shared" ref="J4:J7" ca="1" si="4">"KN" &amp; CHAR(RANDBETWEEN(65,70))</f>
-        <v>KNB</v>
+      <c r="J4" s="13" t="s">
+        <v>54</v>
       </c>
       <c r="K4" s="11">
-        <f t="shared" ref="K4:K7" ca="1" si="5">RANDBETWEEN(30,60)*100</f>
         <v>3900</v>
       </c>
-      <c r="L4" s="5" t="str">
-        <f t="shared" ref="L4:L7" ca="1" si="6">CHOOSE(RANDBETWEEN(1,3),"AC","DC","AC 3Pha")</f>
-        <v>DC</v>
-      </c>
-      <c r="M4" s="16" t="str">
-        <f t="shared" ref="M4:M7" ca="1" si="7">CHOOSE(RANDBETWEEN(1,5),"Lithium-ion","Lead–Acid","Diesel","LPG","Gasoline")</f>
-        <v>Diesel</v>
-      </c>
-      <c r="N4" s="13" t="str">
-        <f t="shared" ref="N4:N7" ca="1" si="8">CHOOSE(RANDBETWEEN(1,2),"Lithium-ion","Lead–Acid")
- &amp; " | " &amp;
-CHOOSE(RANDBETWEEN(1,4),24,36,48,72) &amp; "V"
- &amp; " | " &amp;
-CHOOSE(RANDBETWEEN(1,3),240,360,480) &amp; "Ah"
- &amp; " | " &amp;
-RANDBETWEEN(200,600) &amp; " kg"</f>
-        <v>Lithium-ion | 36V | 360Ah | 358 kg</v>
-      </c>
-      <c r="O4" s="17" t="str">
-        <f t="shared" ref="O4:O7" ca="1" si="9">RANDBETWEEN(1,50) &amp; "A"</f>
-        <v>20A</v>
-      </c>
-      <c r="P4" s="6" t="str">
-        <f t="shared" ref="P4:P7" ca="1" si="10">RANDBETWEEN(600,1200) &amp; " x " &amp; RANDBETWEEN(1000,1500) &amp; "mm"</f>
-        <v>969 x 1496mm</v>
+      <c r="L4" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="M4" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="N4" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="O4" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="Q4" s="5" t="s">
         <v>25</v>
       </c>
       <c r="R4" s="5">
-        <f t="shared" ref="R4:R7" ca="1" si="11">CHOOSE(RANDBETWEEN(1,3), 2, 3, 5)</f>
         <v>3</v>
       </c>
-      <c r="S4" s="5" t="str">
-        <f t="shared" ref="S4:S7" ca="1" si="12">CHOOSE(RANDBETWEEN(1,2),"có","không")</f>
-        <v>có</v>
+      <c r="S4" s="5" t="s">
+        <v>59</v>
       </c>
       <c r="T4" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="U4" s="8" t="str">
-        <f t="shared" ref="U4:U7" ca="1" si="13">CHOOSE(RANDBETWEEN(1,2),"Lốp đặc","Lốp hơi") &amp; ", " &amp;
-ROUND(RAND()*(5-1)+1,1) &amp; "t, " &amp;
-ROUND(RAND()*(6-3)+3,1) &amp; "m, " &amp;
-CHOOSE(RANDBETWEEN(1,3),"Điện","Diesel","Gas") &amp; ", " &amp;
-CHOOSE(RANDBETWEEN(1,2),"Có","Không") &amp; ", " &amp;
-CHOOSE(RANDBETWEEN(1,3),"Mới","Trung bình","Cũ") &amp; ", " &amp;
-RANDBETWEEN(1200,2500) &amp; " x " &amp; RANDBETWEEN(600,1500) &amp; "mm, " &amp;
-ROUND(RAND()*(20-5)+5,1) &amp; "km/h, " &amp;
-ROUND(RAND()*15,1) &amp; "°"</f>
-        <v>Lốp đặc, 3.5t, 3.7m, Điện, Không, Trung bình, 2070 x 1369mm, 16.2km/h, 10.4°</v>
+      <c r="U4" s="8" t="s">
+        <v>60</v>
       </c>
       <c r="V4" s="8" t="s">
         <v>26</v>
       </c>
       <c r="W4" s="21">
-        <f t="shared" ref="W4:W7" ca="1" si="14">RANDBETWEEN(1,5)*10</f>
         <v>10</v>
       </c>
       <c r="X4" s="13">
-        <f t="shared" ref="X4:X7" ca="1" si="15">RANDBETWEEN(16,20)*10</f>
         <v>200</v>
       </c>
       <c r="Y4" s="21">
-        <f t="shared" ref="Y4:Z7" ca="1" si="16">RANDBETWEEN(6,10)*10</f>
         <v>90</v>
       </c>
       <c r="Z4" s="21">
-        <f t="shared" ca="1" si="16"/>
         <v>60</v>
       </c>
-      <c r="AA4" s="14" t="str">
-        <f t="shared" ref="AA4:AA7" ca="1" si="17">"Đại lý_" &amp; CHOOSE(RANDBETWEEN(1,5),"A","B","C","D","E")</f>
-        <v>Đại lý_E</v>
+      <c r="AA4" s="14" t="s">
+        <v>61</v>
       </c>
       <c r="AB4" s="5">
-        <f t="shared" ref="AB4:AB7" ca="1" si="18">RANDBETWEEN(11,15)*10</f>
         <v>150</v>
       </c>
       <c r="AC4" s="5"/>
@@ -1070,9 +1167,8 @@
       <c r="A5" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="13" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>XE_09439</v>
+      <c r="B5" s="13" t="s">
+        <v>62</v>
       </c>
       <c r="C5" s="12">
         <v>45572</v>
@@ -1083,97 +1179,73 @@
       <c r="E5" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>PPT_2</v>
-      </c>
-      <c r="G5" s="13" t="str">
-        <f t="shared" ref="G5:G7" ca="1" si="19">CHOOSE(RANDBETWEEN(1,11),
-"8FB15","8FD25","7FBEU18",
-"FB25-12","FD30T-16",
-"J2.5XN","H3.0FT",
-"FE4P16","FE4P25","FE3D20N")</f>
-        <v>7FBEU18</v>
-      </c>
-      <c r="H5" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>SN-202510-58082</v>
+      <c r="F5" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>65</v>
       </c>
       <c r="I5" s="13">
-        <f t="shared" ca="1" si="3"/>
         <v>2200</v>
       </c>
-      <c r="J5" s="13" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>KNF</v>
+      <c r="J5" s="13" t="s">
+        <v>66</v>
       </c>
       <c r="K5" s="11">
-        <f t="shared" ca="1" si="5"/>
         <v>5400</v>
       </c>
-      <c r="L5" s="5" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v>AC</v>
-      </c>
-      <c r="M5" s="16" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>Lead–Acid</v>
-      </c>
-      <c r="N5" s="13" t="str">
-        <f t="shared" ca="1" si="8"/>
-        <v>Lithium-ion | 36V | 240Ah | 549 kg</v>
-      </c>
-      <c r="O5" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>14A</v>
-      </c>
-      <c r="P5" s="6" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>746 x 1179mm</v>
+      <c r="L5" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="M5" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="N5" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="O5" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="Q5" s="5" t="s">
         <v>25</v>
       </c>
       <c r="R5" s="5">
-        <f t="shared" ca="1" si="11"/>
         <v>3</v>
       </c>
-      <c r="S5" s="5" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>có</v>
+      <c r="S5" s="5" t="s">
+        <v>59</v>
       </c>
       <c r="T5" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="U5" s="8" t="str">
-        <f t="shared" ca="1" si="13"/>
-        <v>Lốp hơi, 1.9t, 3.2m, Gas, Có, Cũ, 1961 x 1353mm, 11.8km/h, 6.8°</v>
+      <c r="U5" s="8" t="s">
+        <v>72</v>
       </c>
       <c r="V5" s="8" t="s">
         <v>26</v>
       </c>
       <c r="W5" s="21">
-        <f t="shared" ca="1" si="14"/>
         <v>20</v>
       </c>
       <c r="X5" s="13">
-        <f t="shared" ca="1" si="15"/>
         <v>170</v>
       </c>
       <c r="Y5" s="21">
-        <f t="shared" ca="1" si="16"/>
         <v>60</v>
       </c>
       <c r="Z5" s="21">
-        <f t="shared" ca="1" si="16"/>
         <v>90</v>
       </c>
-      <c r="AA5" s="14" t="str">
-        <f t="shared" ca="1" si="17"/>
-        <v>Đại lý_A</v>
+      <c r="AA5" s="14" t="s">
+        <v>73</v>
       </c>
       <c r="AB5" s="5">
-        <f t="shared" ca="1" si="18"/>
         <v>110</v>
       </c>
       <c r="AC5" s="5"/>
@@ -1182,9 +1254,8 @@
       <c r="A6" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="13" t="str">
-        <f ca="1">"XE_"&amp;TEXT(RANDBETWEEN(0,99999),"00000")</f>
-        <v>XE_93128</v>
+      <c r="B6" s="13" t="s">
+        <v>74</v>
       </c>
       <c r="C6" s="12">
         <v>45573</v>
@@ -1195,93 +1266,73 @@
       <c r="E6" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>PPT_3</v>
-      </c>
-      <c r="G6" s="13" t="str">
-        <f t="shared" ca="1" si="19"/>
-        <v>H3.0FT</v>
-      </c>
-      <c r="H6" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>SN-202510-62801</v>
+      <c r="F6" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>88</v>
       </c>
       <c r="I6" s="13">
-        <f t="shared" ca="1" si="3"/>
         <v>1600</v>
       </c>
-      <c r="J6" s="13" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>KND</v>
+      <c r="J6" s="13" t="s">
+        <v>75</v>
       </c>
       <c r="K6" s="11">
-        <f t="shared" ca="1" si="5"/>
         <v>6000</v>
       </c>
-      <c r="L6" s="5" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v>AC</v>
-      </c>
-      <c r="M6" s="16" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>Lead–Acid</v>
-      </c>
-      <c r="N6" s="13" t="str">
-        <f t="shared" ca="1" si="8"/>
-        <v>Lithium-ion | 48V | 240Ah | 574 kg</v>
-      </c>
-      <c r="O6" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>8A</v>
-      </c>
-      <c r="P6" s="6" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>1072 x 1484mm</v>
+      <c r="L6" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="M6" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="N6" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="O6" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>78</v>
       </c>
       <c r="Q6" s="5" t="s">
         <v>25</v>
       </c>
       <c r="R6" s="5">
-        <f t="shared" ca="1" si="11"/>
         <v>2</v>
       </c>
-      <c r="S6" s="5" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>không</v>
+      <c r="S6" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="T6" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="U6" s="8" t="str">
-        <f t="shared" ca="1" si="13"/>
-        <v>Lốp hơi, 2.5t, 3.7m, Gas, Có, Mới, 2165 x 1152mm, 7.9km/h, 3.8°</v>
+      <c r="U6" s="8" t="s">
+        <v>79</v>
       </c>
       <c r="V6" s="8" t="s">
         <v>26</v>
       </c>
       <c r="W6" s="21">
-        <f t="shared" ca="1" si="14"/>
         <v>10</v>
       </c>
       <c r="X6" s="13">
-        <f t="shared" ca="1" si="15"/>
         <v>160</v>
       </c>
       <c r="Y6" s="21">
-        <f t="shared" ca="1" si="16"/>
         <v>60</v>
       </c>
       <c r="Z6" s="21">
-        <f t="shared" ca="1" si="16"/>
         <v>100</v>
       </c>
-      <c r="AA6" s="14" t="str">
-        <f t="shared" ca="1" si="17"/>
-        <v>Đại lý_E</v>
+      <c r="AA6" s="14" t="s">
+        <v>61</v>
       </c>
       <c r="AB6" s="5">
-        <f t="shared" ca="1" si="18"/>
         <v>120</v>
       </c>
       <c r="AC6" s="5"/>
@@ -1290,9 +1341,8 @@
       <c r="A7" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="13" t="str">
-        <f ca="1">"XE_"&amp;TEXT(RANDBETWEEN(0,99999),"00000")</f>
-        <v>XE_31056</v>
+      <c r="B7" s="13" t="s">
+        <v>80</v>
       </c>
       <c r="C7" s="12">
         <v>45573</v>
@@ -1303,93 +1353,73 @@
       <c r="E7" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>PPT_4</v>
-      </c>
-      <c r="G7" s="13" t="e">
-        <f t="shared" ca="1" si="19"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H7" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>SN-202510-83707</v>
+      <c r="F7" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>81</v>
       </c>
       <c r="I7" s="13">
-        <f t="shared" ca="1" si="3"/>
         <v>2500</v>
       </c>
-      <c r="J7" s="13" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>KND</v>
+      <c r="J7" s="13" t="s">
+        <v>75</v>
       </c>
       <c r="K7" s="11">
-        <f t="shared" ca="1" si="5"/>
         <v>3500</v>
       </c>
-      <c r="L7" s="5" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v>DC</v>
-      </c>
-      <c r="M7" s="16" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>Lithium-ion</v>
-      </c>
-      <c r="N7" s="13" t="str">
-        <f t="shared" ca="1" si="8"/>
-        <v>Lithium-ion | 72V | 240Ah | 559 kg</v>
-      </c>
-      <c r="O7" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>45A</v>
-      </c>
-      <c r="P7" s="6" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>878 x 1492mm</v>
+      <c r="L7" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="M7" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="N7" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="O7" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="P7" s="6" t="s">
+        <v>85</v>
       </c>
       <c r="Q7" s="5" t="s">
         <v>25</v>
       </c>
       <c r="R7" s="5">
-        <f t="shared" ca="1" si="11"/>
         <v>2</v>
       </c>
-      <c r="S7" s="5" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v>có</v>
+      <c r="S7" s="5" t="s">
+        <v>59</v>
       </c>
       <c r="T7" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="U7" s="8" t="str">
-        <f t="shared" ca="1" si="13"/>
-        <v>Lốp hơi, 4.8t, 4.3m, Gas, Không, Mới, 2489 x 877mm, 8.2km/h, 10.3°</v>
+      <c r="U7" s="8" t="s">
+        <v>86</v>
       </c>
       <c r="V7" s="8" t="s">
         <v>26</v>
       </c>
       <c r="W7" s="21">
-        <f t="shared" ca="1" si="14"/>
         <v>50</v>
       </c>
       <c r="X7" s="13">
-        <f t="shared" ca="1" si="15"/>
         <v>200</v>
       </c>
       <c r="Y7" s="21">
-        <f t="shared" ca="1" si="16"/>
         <v>80</v>
       </c>
       <c r="Z7" s="21">
-        <f t="shared" ca="1" si="16"/>
         <v>60</v>
       </c>
-      <c r="AA7" s="14" t="str">
-        <f t="shared" ca="1" si="17"/>
-        <v>Đại lý_C</v>
+      <c r="AA7" s="14" t="s">
+        <v>87</v>
       </c>
       <c r="AB7" s="5">
-        <f t="shared" ca="1" si="18"/>
         <v>150</v>
       </c>
       <c r="AC7" s="5"/>
@@ -1405,7 +1435,7 @@
     <row r="16" spans="1:29" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="17" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="18" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="19" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="19" ht="13.2" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="20" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="21" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="22" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1896,7 +1926,7 @@
     <row r="507" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="508" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>